<commit_message>
Alle input volgens mij nu gelezen. Classes toegevoegd om dat mogelijk te maken en input files aangepast om het makkelijker te maken
</commit_message>
<xml_diff>
--- a/inputs/docenteninfo.xlsx
+++ b/inputs/docenteninfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="3340" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>naam</t>
   </si>
@@ -39,9 +39,6 @@
     <t>GB</t>
   </si>
   <si>
-    <t>wiskunde</t>
-  </si>
-  <si>
     <t>A. van Willigen</t>
   </si>
   <si>
@@ -54,39 +51,12 @@
     <t>AT</t>
   </si>
   <si>
-    <t>maatschappijleer</t>
-  </si>
-  <si>
     <t>F. van Harmelen</t>
   </si>
   <si>
     <t>FH</t>
   </si>
   <si>
-    <t>aardrijkskunde</t>
-  </si>
-  <si>
-    <t>gymnastiek</t>
-  </si>
-  <si>
-    <t>handenarbeid</t>
-  </si>
-  <si>
-    <t>nederlands</t>
-  </si>
-  <si>
-    <t>latijn|grieks</t>
-  </si>
-  <si>
-    <t>geschiedenis</t>
-  </si>
-  <si>
-    <t>biologie</t>
-  </si>
-  <si>
-    <t>engels</t>
-  </si>
-  <si>
     <t>AB</t>
   </si>
   <si>
@@ -157,16 +127,65 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>LA|GR</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>ML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,14 +208,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,7 +552,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,19 +577,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -577,246 +600,287 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1">
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1">
         <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
         <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1">
         <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1">
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="1">
         <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1">
         <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
hoera, alle input wordt gelezen! geloof ik! maar toch!
</commit_message>
<xml_diff>
--- a/inputs/docenteninfo.xlsx
+++ b/inputs/docenteninfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="9380" yWindow="1060" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>naam</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>ML</t>
+  </si>
+  <si>
+    <t>A. Noniem</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>FA</t>
   </si>
 </sst>
 </file>
@@ -549,21 +558,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -875,6 +886,32 @@
         <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>